<commit_message>
menu analisis dan update database
</commit_message>
<xml_diff>
--- a/Data CSV/Data_lengkap Tahun 2023.xlsx
+++ b/Data CSV/Data_lengkap Tahun 2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELAINE\ta_elaine\Data CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E38175-F4E3-49C7-A104-14656D6D5B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE6F02E-88AB-48FE-B73C-7192E739B1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12510" yWindow="1665" windowWidth="26610" windowHeight="14205" xr2:uid="{3E2A20D6-75D5-4D9C-811B-0EA86BE7BAC5}"/>
+    <workbookView xWindow="3900" yWindow="2130" windowWidth="14085" windowHeight="13155" xr2:uid="{3E2A20D6-75D5-4D9C-811B-0EA86BE7BAC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -63,6 +63,105 @@
   </si>
   <si>
     <t>Kementerian Koordinator Bidang Politik, Hukum dan Keamanan</t>
+  </si>
+  <si>
+    <t>Kementerian Koordinator Bidang Perekonomian</t>
+  </si>
+  <si>
+    <t>Kementerian Koordinator Bidang Pembangunan Manusia dan Kebudayaan</t>
+  </si>
+  <si>
+    <t>Kementerian Koordinator Bidang Kemaritiman</t>
+  </si>
+  <si>
+    <t>Kementerian Koperasi dan Usaha Kecil dan Menengah</t>
+  </si>
+  <si>
+    <t>Kementerian Badan Usaha Milik Negara</t>
+  </si>
+  <si>
+    <t>Kementerian Pemberdayaan Perempuan dan Perlindungan Anak</t>
+  </si>
+  <si>
+    <t>Kementerian Pendayagunaan Aparatur Negara dan Reformasi Birokrasi</t>
+  </si>
+  <si>
+    <t>Kementerian Pemuda dan Olahraga</t>
+  </si>
+  <si>
+    <t>Kementerian Desa, Pembangunan Daerah Tertinggal dan Transmigrasi</t>
+  </si>
+  <si>
+    <t>Kementerian Dalam Negeri</t>
+  </si>
+  <si>
+    <t>Kementerian Luar Negeri</t>
+  </si>
+  <si>
+    <t>Kementerian Pertahanan</t>
+  </si>
+  <si>
+    <t>Kementerian Hukum dan Hak Asasi Manusia</t>
+  </si>
+  <si>
+    <t>Kementerian Keuangan</t>
+  </si>
+  <si>
+    <t>Kementerian Pertanian</t>
+  </si>
+  <si>
+    <t>Kementerian Energi dan Sumber Daya Mineral</t>
+  </si>
+  <si>
+    <t>Kementerian Perhubungan</t>
+  </si>
+  <si>
+    <t>Kementerian Pendidikan dan Kebudayaan</t>
+  </si>
+  <si>
+    <t>Kementerian Kesehatan</t>
+  </si>
+  <si>
+    <t>Kementerian Agama</t>
+  </si>
+  <si>
+    <t>Kementerian Ketenagakerjaan</t>
+  </si>
+  <si>
+    <t>Kementerian Sosial</t>
+  </si>
+  <si>
+    <t>Kementerian Lingkungan Hidup dan Kehutanan</t>
+  </si>
+  <si>
+    <t>Kementerian Kelautan dan Perikanan</t>
+  </si>
+  <si>
+    <t>Kementerian Komunikasi dan Informatika</t>
+  </si>
+  <si>
+    <t>Kementerian Perdagangan</t>
+  </si>
+  <si>
+    <t>Kementerian Perindustrian</t>
+  </si>
+  <si>
+    <t>Kementerian Pekerjaan Umum &amp; Perumahan Rakyat</t>
+  </si>
+  <si>
+    <t>Kementerian Pariwisata dan Ekonomi Kreatif/Badan Pariwisata dan Ekonomi Kreatif</t>
+  </si>
+  <si>
+    <t>Kementerian Sekretariat Negara</t>
+  </si>
+  <si>
+    <t>Kementerian Perencanaan Pembangunan Nasional/Badan Perencanaan Pembangunan Nasional</t>
+  </si>
+  <si>
+    <t>Kementerian Investasi/Badan Koordinasi Penanaman Modal</t>
+  </si>
+  <si>
+    <t>Kementerian Agraria dan Tata Ruang/Badan Pertanahan Nasional</t>
   </si>
 </sst>
 </file>
@@ -9978,15 +10077,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94BB4416-E7DC-48C9-AF74-C94A75507DE7}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10037,6 +10136,798 @@
         <v>3.74</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B3,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600078</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>3.72</v>
+      </c>
+      <c r="D3">
+        <v>3.3</v>
+      </c>
+      <c r="E3">
+        <v>3.4</v>
+      </c>
+      <c r="F3">
+        <v>2.91</v>
+      </c>
+      <c r="G3">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B4,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>3.13</v>
+      </c>
+      <c r="D4">
+        <v>3.1</v>
+      </c>
+      <c r="E4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B5,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600079</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>3.31</v>
+      </c>
+      <c r="D5">
+        <v>3.1</v>
+      </c>
+      <c r="E5">
+        <v>3.1</v>
+      </c>
+      <c r="F5">
+        <v>2.73</v>
+      </c>
+      <c r="G5">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B6,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>3.5</v>
+      </c>
+      <c r="D6">
+        <v>3.9</v>
+      </c>
+      <c r="E6">
+        <v>3.3</v>
+      </c>
+      <c r="F6">
+        <v>2.82</v>
+      </c>
+      <c r="G6">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B7,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600080</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>4.41</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F7">
+        <v>3.82</v>
+      </c>
+      <c r="G7">
+        <v>4.63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B8,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600003</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>3.41</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2.4</v>
+      </c>
+      <c r="F8">
+        <v>2.73</v>
+      </c>
+      <c r="G8">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B9,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600081</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>3.97</v>
+      </c>
+      <c r="D9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E9">
+        <v>3.7</v>
+      </c>
+      <c r="F9">
+        <v>3.82</v>
+      </c>
+      <c r="G9">
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B10,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600314</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>3.35</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>2.7</v>
+      </c>
+      <c r="F10">
+        <v>2.27</v>
+      </c>
+      <c r="G10">
+        <v>3.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B11,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600082</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>3.87</v>
+      </c>
+      <c r="D11">
+        <v>3.7</v>
+      </c>
+      <c r="E11">
+        <v>3.8</v>
+      </c>
+      <c r="F11">
+        <v>3.09</v>
+      </c>
+      <c r="G11">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B12,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600004</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>3.64</v>
+      </c>
+      <c r="D12">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E12">
+        <v>3.4</v>
+      </c>
+      <c r="F12">
+        <v>2.27</v>
+      </c>
+      <c r="G12">
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B13,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600005</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>3.26</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>3.9</v>
+      </c>
+      <c r="F13">
+        <v>1.18</v>
+      </c>
+      <c r="G13">
+        <v>4.0199999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B14,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600315</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>3.43</v>
+      </c>
+      <c r="D14">
+        <v>3.1</v>
+      </c>
+      <c r="E14">
+        <v>3.4</v>
+      </c>
+      <c r="F14">
+        <v>3.18</v>
+      </c>
+      <c r="G14">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B15,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600006</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>4.21</v>
+      </c>
+      <c r="D15">
+        <v>3.8</v>
+      </c>
+      <c r="E15">
+        <v>3.9</v>
+      </c>
+      <c r="F15">
+        <v>2.82</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B16,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600083</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>4.66</v>
+      </c>
+      <c r="D16">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E16">
+        <v>4.7</v>
+      </c>
+      <c r="F16">
+        <v>4.18</v>
+      </c>
+      <c r="G16">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B17,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600007</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>3.86</v>
+      </c>
+      <c r="D17">
+        <v>3.4</v>
+      </c>
+      <c r="E17">
+        <v>3.7</v>
+      </c>
+      <c r="F17">
+        <v>2.36</v>
+      </c>
+      <c r="G17">
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B18,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600008</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>3.52</v>
+      </c>
+      <c r="D18">
+        <v>4.7</v>
+      </c>
+      <c r="E18">
+        <v>3.5</v>
+      </c>
+      <c r="F18">
+        <v>1.36</v>
+      </c>
+      <c r="G18">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B19,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600009</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>3.71</v>
+      </c>
+      <c r="D19">
+        <v>4.2</v>
+      </c>
+      <c r="E19">
+        <v>3.7</v>
+      </c>
+      <c r="F19">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="G19">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B20,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600084</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>3.9</v>
+      </c>
+      <c r="D20">
+        <v>3.3</v>
+      </c>
+      <c r="E20">
+        <v>3.9</v>
+      </c>
+      <c r="F20">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="G20">
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B21,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600085</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>3.31</v>
+      </c>
+      <c r="D21">
+        <v>2.6</v>
+      </c>
+      <c r="E21">
+        <v>3.7</v>
+      </c>
+      <c r="F21">
+        <v>2.64</v>
+      </c>
+      <c r="G21">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B22,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600086</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>3.58</v>
+      </c>
+      <c r="D22">
+        <v>3.4</v>
+      </c>
+      <c r="E22">
+        <v>3.3</v>
+      </c>
+      <c r="F22">
+        <v>2.27</v>
+      </c>
+      <c r="G22">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B23,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600010</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>3.27</v>
+      </c>
+      <c r="D23">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E23">
+        <v>3.2</v>
+      </c>
+      <c r="F23">
+        <v>1.55</v>
+      </c>
+      <c r="G23">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B24,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600087</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24">
+        <v>3.04</v>
+      </c>
+      <c r="D24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E24">
+        <v>2.8</v>
+      </c>
+      <c r="F24">
+        <v>1.73</v>
+      </c>
+      <c r="G24">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B25,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600088</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>3.62</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>3.2</v>
+      </c>
+      <c r="F25">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="G25">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B26,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600089</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26">
+        <v>3.58</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>3.1</v>
+      </c>
+      <c r="F26">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="G26">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B27,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600090</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>4.2</v>
+      </c>
+      <c r="F27">
+        <v>3.27</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B28,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600011</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28">
+        <v>4.16</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F28">
+        <v>3.18</v>
+      </c>
+      <c r="G28">
+        <v>4.1399999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B29,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600316</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
+        <v>2.89</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>1.9</v>
+      </c>
+      <c r="F29">
+        <v>1.36</v>
+      </c>
+      <c r="G29">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B30,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600091</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>3.81</v>
+      </c>
+      <c r="D30">
+        <v>4.5</v>
+      </c>
+      <c r="E30">
+        <v>3.5</v>
+      </c>
+      <c r="F30">
+        <v>1.27</v>
+      </c>
+      <c r="G30">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B31,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600092</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>4.67</v>
+      </c>
+      <c r="D31">
+        <v>4.8</v>
+      </c>
+      <c r="E31">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F31">
+        <v>4.45</v>
+      </c>
+      <c r="G31">
+        <v>4.76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B32,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600093</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32">
+        <v>3.38</v>
+      </c>
+      <c r="D32">
+        <v>3.1</v>
+      </c>
+      <c r="E32">
+        <v>3.4</v>
+      </c>
+      <c r="F32">
+        <v>2.09</v>
+      </c>
+      <c r="G32">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B33,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600102</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="D33">
+        <v>4.2</v>
+      </c>
+      <c r="E33">
+        <v>3.6</v>
+      </c>
+      <c r="F33">
+        <v>3.36</v>
+      </c>
+      <c r="G33">
+        <v>4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B34,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600106</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34">
+        <v>2.83</v>
+      </c>
+      <c r="D34">
+        <v>2.1</v>
+      </c>
+      <c r="E34">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F34">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G34">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>INDEX('[1]instansi pusat'!$A$1:$D$1000,MATCH(B35,'[1]instansi pusat'!$D$1:$D$1000,0),1)</f>
+        <v>i2023110600014</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>3.95</v>
+      </c>
+      <c r="D35">
+        <v>4.2</v>
+      </c>
+      <c r="E35">
+        <v>3.6</v>
+      </c>
+      <c r="F35">
+        <v>3.45</v>
+      </c>
+      <c r="G35">
+        <v>4.26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>